<commit_message>
Removed some files, updated some charts
</commit_message>
<xml_diff>
--- a/Complexity.xlsx
+++ b/Complexity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="38400" windowHeight="20380" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="38080" yWindow="460" windowWidth="38400" windowHeight="20380" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="2x2 Grid" sheetId="6" r:id="rId1"/>
@@ -87,10 +87,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,8 +155,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -158,10 +176,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -230,14 +260,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>2x2</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Grid, Complexity vs Nodes Evaluated</a:t>
+              <a:t>2x2 Grid, Complexity vs Nodes Evaluated</a:t>
             </a:r>
             <a:endParaRPr lang="en-US">
               <a:effectLst/>
@@ -1166,7 +1192,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Complexity (Nodes Evalutated)</a:t>
+                  <a:t> Complexity (Nodes Evaluated)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -3090,7 +3116,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Complexity (Nodes Evaluted)</a:t>
+                  <a:t> Complexity (Nodes Evaluated)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -3647,6 +3673,24 @@
                 <c:pt idx="14">
                   <c:v>3.477998E6</c:v>
                 </c:pt>
+                <c:pt idx="15">
+                  <c:v>401771.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.850497E6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.525015E6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.0034696E7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.815947E6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>826179.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -4142,12 +4186,14 @@
         <c:crossAx val="386560288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2.0"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="386560288"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
+          <c:min val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -16994,6 +17040,7 @@
     <sheetView zoomScale="169" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </chartsheet>
 </file>
@@ -18707,8 +18754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19255,8 +19302,12 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="E18" s="2">
+        <v>401771</v>
+      </c>
+      <c r="F18" s="2">
+        <v>401771</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="6">
@@ -19275,8 +19326,12 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="E19" s="2">
+        <v>3850497</v>
+      </c>
+      <c r="F19" s="2">
+        <v>3850497</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="6">
@@ -19295,8 +19350,12 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="2">
+        <v>2525015</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2525015</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="6">
@@ -19315,8 +19374,12 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="E21" s="2">
+        <v>20034696</v>
+      </c>
+      <c r="F21" s="2">
+        <v>20034696</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="6">
@@ -19335,8 +19398,12 @@
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="E22" s="2">
+        <v>3815947</v>
+      </c>
+      <c r="F22" s="2">
+        <v>3815947</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="6">
@@ -19355,8 +19422,12 @@
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="E23" s="2">
+        <v>826179</v>
+      </c>
+      <c r="F23" s="2">
+        <v>826179</v>
+      </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="6">
@@ -19389,8 +19460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H518"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="F197" sqref="F197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23942,6 +24013,10 @@
       </c>
     </row>
     <row r="203" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="F203">
+        <f>MAX(F3:F202)</f>
+        <v>151</v>
+      </c>
       <c r="G203">
         <v>781810</v>
       </c>
@@ -26477,10 +26552,11 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D190">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>D2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>